<commit_message>
R Program Update for Control
Fixed up the control program. I will be working on the treatment and analysis portions in the coming days.
</commit_message>
<xml_diff>
--- a/thread_strength/summarized_data/integral_control.xlsx
+++ b/thread_strength/summarized_data/integral_control.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t xml:space="preserve">mussel</t>
   </si>
@@ -23,10 +23,109 @@
     <t xml:space="preserve">auc</t>
   </si>
   <si>
+    <t xml:space="preserve">G28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T57</t>
+  </si>
+  <si>
     <t xml:space="preserve">T58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02</t>
   </si>
 </sst>
 </file>
@@ -377,6 +476,930 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
+        <v>0.179692984150595</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.263125001024581</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.076540570393249</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.273339213133971</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.0198953133919</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.37170250944692</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.11253549259134</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.193543468727241</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1.80411237261945</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.242976153060752</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.58103712528359</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.443745404510893</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.430585407686116</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.135134717160769</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.240439515047792</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.245523064488185</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.69061345527425</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.756023435014641</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.667967817281106</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.370682392918067</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.273708887798214</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.378439447746792</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="n">
+        <v>2.00004119269248</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.793496655657292</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.210420092922101</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.523464111794872</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.28805482522275</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.492934599061512</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.10148659852088</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.084310382573428</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.0350850902805546</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.234471403738663</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.245195530451986</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.980721331522084</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1.47077025787491</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.519898390909091</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1.70848243847461</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" t="n">
+        <v>2.18664563295616</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.293875228576557</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1.00688152957746</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1.24731350665164</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.276504183357356</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.558608817499495</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.474241506525802</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.398586843224299</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.348496204103527</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.295518097018083</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.0761787722842886</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1.22766333739364</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.406050352156382</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.223449965454546</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.465963966351108</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.108715163303903</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.0558033366446877</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.49618739375</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.35888822589895</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.205269372433868</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.33259011499748</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.0877670378204362</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.363457821476744</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1.14876421202948</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.706422700653736</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.432382347470233</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.790233693737491</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>29</v>
+      </c>
+      <c r="B66" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.730729305649718</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.9958893292062</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.642948030883435</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" t="n">
+        <v>1.42485930727701</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.390346603563956</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>31</v>
+      </c>
+      <c r="B71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.053723863768116</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.157390608443112</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>32</v>
+      </c>
+      <c r="B73" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" t="n">
+        <v>1.05138779714286</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>33</v>
+      </c>
+      <c r="B74" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.0851419529793792</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.201476578017984</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>33</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.349384981985005</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>34</v>
+      </c>
+      <c r="B77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.615000840103553</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>34</v>
+      </c>
+      <c r="B78" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.828555419446155</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>35</v>
+      </c>
+      <c r="B79" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.0652454959277768</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>35</v>
+      </c>
+      <c r="B80" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.343399704639175</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>35</v>
+      </c>
+      <c r="B81" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.336737629252917</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>36</v>
+      </c>
+      <c r="B82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.197904608287293</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>36</v>
+      </c>
+      <c r="B83" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.186071436082481</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>36</v>
+      </c>
+      <c r="B84" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.0455081681339704</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>37</v>
+      </c>
+      <c r="B85" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.23514499058402</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B86" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" t="n">
         <v>0.322754007773647</v>
       </c>
     </row>

</xml_diff>